<commit_message>
Fills out excel chart up to 2^14
</commit_message>
<xml_diff>
--- a/SortingTimes.xlsx
+++ b/SortingTimes.xlsx
@@ -142,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -183,6 +183,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,11 +491,12 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -539,10 +543,18 @@
         <v>9</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="15">
+        <v>1.4518000000000001E-5</v>
+      </c>
+      <c r="D3" s="15">
+        <v>3.8627900000000001E-4</v>
+      </c>
+      <c r="E3" s="3">
+        <v>4.2885777E-2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.55967043999999999</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="1">
         <v>514.70000000000005</v>
@@ -553,10 +565,18 @@
         <v>10</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="15">
+        <v>1.4518000000000001E-5</v>
+      </c>
+      <c r="D4" s="15">
+        <v>3.8275899999999999E-4</v>
+      </c>
+      <c r="E4" s="3">
+        <v>8.6217670000000007E-3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.49969819199999999</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="1">
         <v>549.84</v>
@@ -567,10 +587,18 @@
         <v>11</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="15">
+        <v>1.6279000000000001E-5</v>
+      </c>
+      <c r="D5" s="15">
+        <v>3.8363900000000002E-4</v>
+      </c>
+      <c r="E5" s="3">
+        <v>9.4787959999999994E-3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.51871341699999995</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="1">
         <v>547.01</v>
@@ -617,10 +645,18 @@
         <v>9</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="C9" s="15">
+        <v>1.3638999999999999E-5</v>
+      </c>
+      <c r="D9" s="15">
+        <v>3.58122E-4</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7.4994459999999999E-3</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.55831010400000003</v>
+      </c>
       <c r="G9" s="3"/>
       <c r="H9" s="1">
         <v>542.5</v>
@@ -631,10 +667,18 @@
         <v>10</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="C10" s="15">
+        <v>1.4078E-5</v>
+      </c>
+      <c r="D10" s="15">
+        <v>3.5944200000000002E-4</v>
+      </c>
+      <c r="E10" s="3">
+        <v>7.2961880000000003E-3</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.54835307899999997</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="1">
         <v>551.22</v>
@@ -645,10 +689,18 @@
         <v>11</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="C11" s="15">
+        <v>1.4079E-5</v>
+      </c>
+      <c r="D11" s="15">
+        <v>3.5856199999999999E-4</v>
+      </c>
+      <c r="E11" s="3">
+        <v>7.609874E-3</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.51842172900000005</v>
+      </c>
       <c r="G11" s="3"/>
       <c r="H11" s="1">
         <v>519.66</v>
@@ -665,8 +717,8 @@
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="1">
-        <f>H18</f>
-        <v>0.18333333333333335</v>
+        <f>AVERAGE(H9:H11)</f>
+        <v>537.79333333333341</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -695,10 +747,18 @@
         <v>9</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="C15" s="15">
+        <v>3.3436000000000003E-5</v>
+      </c>
+      <c r="D15" s="15">
+        <v>2.88609E-4</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2.453621E-3</v>
+      </c>
+      <c r="F15" s="3">
+        <v>7.8940840000000009E-3</v>
+      </c>
       <c r="G15" s="3"/>
       <c r="H15" s="1">
         <v>0.18</v>
@@ -709,10 +769,18 @@
         <v>10</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="C16" s="15">
+        <v>3.2557E-5</v>
+      </c>
+      <c r="D16" s="15">
+        <v>2.6397200000000001E-4</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1.839006E-3</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2.6222981999999999E-2</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="1">
         <v>0.18</v>
@@ -723,10 +791,18 @@
         <v>11</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="C17" s="15">
+        <v>3.2555999999999998E-5</v>
+      </c>
+      <c r="D17" s="15">
+        <v>2.7233100000000001E-4</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1.7254970000000001E-3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>8.5971290000000002E-3</v>
+      </c>
       <c r="G17" s="3"/>
       <c r="H17" s="1">
         <v>0.19</v>

</xml_diff>

<commit_message>
Finish value inputs for 2^17
</commit_message>
<xml_diff>
--- a/SortingTimes.xlsx
+++ b/SortingTimes.xlsx
@@ -16,12 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Sorting Method</t>
-  </si>
-  <si>
-    <t>n</t>
   </si>
   <si>
     <t>2^4</t>
@@ -488,23 +485,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -522,304 +519,302 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>8</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1.4518000000000001E-5</v>
+      </c>
+      <c r="C3" s="15">
+        <v>3.8627900000000001E-4</v>
+      </c>
+      <c r="D3" s="3">
+        <v>8.8540619999999993E-3</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.55967043999999999</v>
+      </c>
+      <c r="F3" s="3">
+        <v>31.472796802000001</v>
+      </c>
+      <c r="G3" s="1">
+        <v>514.70000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="15">
+      <c r="B4" s="15">
         <v>1.4518000000000001E-5</v>
       </c>
-      <c r="D3" s="15">
-        <v>3.8627900000000001E-4</v>
-      </c>
-      <c r="E3" s="3">
-        <v>4.2885777E-2</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.55967043999999999</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="1">
-        <v>514.70000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="C4" s="15">
+        <v>3.8275899999999999E-4</v>
+      </c>
+      <c r="D4" s="3">
+        <v>8.6217670000000007E-3</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.49969819199999999</v>
+      </c>
+      <c r="F4" s="3">
+        <v>31.899376058000001</v>
+      </c>
+      <c r="G4" s="1">
+        <v>549.84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="15">
-        <v>1.4518000000000001E-5</v>
-      </c>
-      <c r="D4" s="15">
-        <v>3.8275899999999999E-4</v>
-      </c>
-      <c r="E4" s="3">
-        <v>8.6217670000000007E-3</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.49969819199999999</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="1">
-        <v>549.84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="15">
+        <v>1.6279000000000001E-5</v>
+      </c>
       <c r="C5" s="15">
-        <v>1.6279000000000001E-5</v>
-      </c>
-      <c r="D5" s="15">
         <v>3.8363900000000002E-4</v>
       </c>
+      <c r="D5" s="3">
+        <v>9.4787959999999994E-3</v>
+      </c>
       <c r="E5" s="3">
-        <v>9.4787959999999994E-3</v>
+        <v>0.51871341699999995</v>
       </c>
       <c r="F5" s="3">
-        <v>0.51871341699999995</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="1">
+        <v>31.486772361</v>
+      </c>
+      <c r="G5" s="1">
         <v>547.01</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="1">
-        <f>AVERAGE(H3:H5)</f>
+      <c r="G6" s="1">
+        <f>AVERAGE(G3:G5)</f>
         <v>537.18333333333328</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15">
+        <v>1.3638999999999999E-5</v>
+      </c>
+      <c r="C9" s="15">
+        <v>3.58122E-4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>7.4994459999999999E-3</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.55831010400000003</v>
+      </c>
+      <c r="F9" s="3">
+        <v>32.668425161000002</v>
+      </c>
+      <c r="G9" s="1">
+        <v>542.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="15">
-        <v>1.3638999999999999E-5</v>
-      </c>
-      <c r="D9" s="15">
-        <v>3.58122E-4</v>
-      </c>
-      <c r="E9" s="3">
-        <v>7.4994459999999999E-3</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.55831010400000003</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="1">
-        <v>542.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="B10" s="15">
+        <v>1.4078E-5</v>
+      </c>
+      <c r="C10" s="15">
+        <v>3.5944200000000002E-4</v>
+      </c>
+      <c r="D10" s="3">
+        <v>7.2961880000000003E-3</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.54835307899999997</v>
+      </c>
+      <c r="F10" s="3">
+        <v>31.550679991999999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>551.22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="15">
-        <v>1.4078E-5</v>
-      </c>
-      <c r="D10" s="15">
-        <v>3.5944200000000002E-4</v>
-      </c>
-      <c r="E10" s="3">
-        <v>7.2961880000000003E-3</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.54835307899999997</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="1">
-        <v>551.22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="15">
+        <v>1.4079E-5</v>
+      </c>
       <c r="C11" s="15">
-        <v>1.4079E-5</v>
-      </c>
-      <c r="D11" s="15">
         <v>3.5856199999999999E-4</v>
       </c>
+      <c r="D11" s="3">
+        <v>7.609874E-3</v>
+      </c>
       <c r="E11" s="3">
-        <v>7.609874E-3</v>
+        <v>0.51842172900000005</v>
       </c>
       <c r="F11" s="3">
-        <v>0.51842172900000005</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="1">
+        <v>31.671601184</v>
+      </c>
+      <c r="G11" s="1">
         <v>519.66</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="1">
-        <f>AVERAGE(H9:H11)</f>
+      <c r="G12" s="1">
+        <f>AVERAGE(G9:G11)</f>
         <v>537.79333333333341</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="15">
+        <v>3.3436000000000003E-5</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2.88609E-4</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2.453621E-3</v>
+      </c>
+      <c r="E15" s="3">
+        <v>7.8940840000000009E-3</v>
+      </c>
+      <c r="F15" s="3">
+        <v>4.8886302E-2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="15">
-        <v>3.3436000000000003E-5</v>
-      </c>
-      <c r="D15" s="15">
-        <v>2.88609E-4</v>
-      </c>
-      <c r="E15" s="3">
-        <v>2.453621E-3</v>
-      </c>
-      <c r="F15" s="3">
-        <v>7.8940840000000009E-3</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="1">
+      <c r="B16" s="15">
+        <v>3.2557E-5</v>
+      </c>
+      <c r="C16" s="15">
+        <v>2.6397200000000001E-4</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1.839006E-3</v>
+      </c>
+      <c r="E16" s="3">
+        <v>8.9609700000000004E-3</v>
+      </c>
+      <c r="F16" s="3">
+        <v>4.7949200999999997E-2</v>
+      </c>
+      <c r="G16" s="1">
         <v>0.18</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="15">
-        <v>3.2557E-5</v>
-      </c>
-      <c r="D16" s="15">
-        <v>2.6397200000000001E-4</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1.839006E-3</v>
-      </c>
-      <c r="F16" s="3">
-        <v>2.6222981999999999E-2</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="1">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="15">
+        <v>3.2555999999999998E-5</v>
+      </c>
       <c r="C17" s="15">
-        <v>3.2555999999999998E-5</v>
-      </c>
-      <c r="D17" s="15">
         <v>2.7233100000000001E-4</v>
       </c>
+      <c r="D17" s="3">
+        <v>1.7254970000000001E-3</v>
+      </c>
       <c r="E17" s="3">
-        <v>1.7254970000000001E-3</v>
+        <v>8.5971290000000002E-3</v>
       </c>
       <c r="F17" s="3">
-        <v>8.5971290000000002E-3</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="1">
+        <v>4.7803576E-2</v>
+      </c>
+      <c r="G17" s="1">
         <v>0.19</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="1">
-        <f>AVERAGE(H15:H17)</f>
+      <c r="G18" s="1">
+        <f>AVERAGE(G15:G17)</f>
         <v>0.18333333333333335</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Creates comment shells, removes some values from SortingTimes
</commit_message>
<xml_diff>
--- a/SortingTimes.xlsx
+++ b/SortingTimes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="17235" windowHeight="6210"/>
@@ -11,28 +11,19 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Sorting Method</t>
   </si>
   <si>
-    <t>2^4</t>
-  </si>
-  <si>
     <t>2^7</t>
   </si>
   <si>
-    <t>2^10</t>
-  </si>
-  <si>
-    <t>2^14</t>
-  </si>
-  <si>
     <t>2^17</t>
   </si>
   <si>
@@ -58,13 +49,28 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>2^5</t>
+  </si>
+  <si>
+    <t>2^9</t>
+  </si>
+  <si>
+    <t>2^11</t>
+  </si>
+  <si>
+    <t>2^13</t>
+  </si>
+  <si>
+    <t>2^15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +118,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -139,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -178,12 +192,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,342 +504,327 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="15">
-        <v>1.4518000000000001E-5</v>
-      </c>
-      <c r="C3" s="15">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14">
         <v>3.8627900000000001E-4</v>
       </c>
-      <c r="D3" s="3">
-        <v>8.8540619999999993E-3</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.55967043999999999</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="3">
         <v>31.472796802000001</v>
       </c>
-      <c r="G3" s="1">
+      <c r="I3" s="1">
         <v>514.70000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="15">
-        <v>1.4518000000000001E-5</v>
-      </c>
-      <c r="C4" s="15">
+        <v>6</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14">
         <v>3.8275899999999999E-4</v>
       </c>
-      <c r="D4" s="3">
-        <v>8.6217670000000007E-3</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.49969819199999999</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="3">
         <v>31.899376058000001</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I4" s="1">
         <v>549.84</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14">
+        <v>3.8363900000000002E-4</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="3">
+        <v>31.486772361</v>
+      </c>
+      <c r="I5" s="1">
+        <v>547.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="15">
-        <v>1.6279000000000001E-5</v>
-      </c>
-      <c r="C5" s="15">
-        <v>3.8363900000000002E-4</v>
-      </c>
-      <c r="D5" s="3">
-        <v>9.4787959999999994E-3</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.51871341699999995</v>
-      </c>
-      <c r="F5" s="3">
-        <v>31.486772361</v>
-      </c>
-      <c r="G5" s="1">
-        <v>547.01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="1">
-        <f>AVERAGE(G3:G5)</f>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="17">
+        <f>AVERAGE(I3:I5)</f>
         <v>537.18333333333328</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="15">
-        <v>1.3638999999999999E-5</v>
-      </c>
-      <c r="C9" s="15">
+        <v>5</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14">
         <v>3.58122E-4</v>
       </c>
-      <c r="D9" s="3">
-        <v>7.4994459999999999E-3</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.55831010400000003</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="3">
         <v>32.668425161000002</v>
       </c>
-      <c r="G9" s="1">
+      <c r="I9" s="1">
         <v>542.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="15">
-        <v>1.4078E-5</v>
-      </c>
-      <c r="C10" s="15">
+        <v>6</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14">
         <v>3.5944200000000002E-4</v>
       </c>
-      <c r="D10" s="3">
-        <v>7.2961880000000003E-3</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.54835307899999997</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="3">
         <v>31.550679991999999</v>
       </c>
-      <c r="G10" s="1">
+      <c r="I10" s="1">
         <v>551.22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14">
+        <v>3.5856199999999999E-4</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="3">
+        <v>31.671601184</v>
+      </c>
+      <c r="I11" s="1">
+        <v>519.66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>10</v>
-      </c>
-      <c r="B11" s="15">
-        <v>1.4079E-5</v>
-      </c>
-      <c r="C11" s="15">
-        <v>3.5856199999999999E-4</v>
-      </c>
-      <c r="D11" s="3">
-        <v>7.609874E-3</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.51842172900000005</v>
-      </c>
-      <c r="F11" s="3">
-        <v>31.671601184</v>
-      </c>
-      <c r="G11" s="1">
-        <v>519.66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>13</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="1">
-        <f>AVERAGE(G9:G11)</f>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="17">
+        <f>AVERAGE(I9:I11)</f>
         <v>537.79333333333341</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="15">
-        <v>3.3436000000000003E-5</v>
-      </c>
-      <c r="C15" s="15">
+        <v>5</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14">
         <v>2.88609E-4</v>
       </c>
-      <c r="D15" s="3">
-        <v>2.453621E-3</v>
-      </c>
-      <c r="E15" s="3">
-        <v>7.8940840000000009E-3</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="3">
         <v>4.8886302E-2</v>
       </c>
-      <c r="G15" s="1">
+      <c r="I15" s="1">
         <v>0.18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="15">
-        <v>3.2557E-5</v>
-      </c>
-      <c r="C16" s="15">
+        <v>6</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14">
         <v>2.6397200000000001E-4</v>
       </c>
-      <c r="D16" s="3">
-        <v>1.839006E-3</v>
-      </c>
-      <c r="E16" s="3">
-        <v>8.9609700000000004E-3</v>
-      </c>
-      <c r="F16" s="3">
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="3">
         <v>4.7949200999999997E-2</v>
       </c>
-      <c r="G16" s="1">
+      <c r="I16" s="1">
         <v>0.18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14">
+        <v>2.7233100000000001E-4</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="3">
+        <v>4.7803576E-2</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="15">
-        <v>3.2555999999999998E-5</v>
-      </c>
-      <c r="C17" s="15">
-        <v>2.7233100000000001E-4</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1.7254970000000001E-3</v>
-      </c>
-      <c r="E17" s="3">
-        <v>8.5971290000000002E-3</v>
-      </c>
-      <c r="F17" s="3">
-        <v>4.7803576E-2</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="1">
-        <f>AVERAGE(G15:G17)</f>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17">
+        <f>AVERAGE(I15:I17)</f>
         <v>0.18333333333333335</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Finishes collecting data, finishes charts
</commit_message>
<xml_diff>
--- a/SortingTimes.xlsx
+++ b/SortingTimes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="17235" windowHeight="6210"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -153,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -173,9 +173,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -198,7 +195,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -215,6 +211,705 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Sorting</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Algorithm Times: 2^5 to 2^11</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14328018372703413"/>
+          <c:y val="0.10855505527819392"/>
+          <c:w val="0.65119160104986873"/>
+          <c:h val="0.7667434357266607"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Method 1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2^5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.035666666666667E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8422566666666667E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.814410333333333E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2528693666666665E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Method 2</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2^5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.0356999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5870866666666665E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2819196666666667E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6679654333333334E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Method 3</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2^5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.5790999999999992E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7497066666666667E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6031903333333334E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9214230000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="85671296"/>
+        <c:axId val="91909120"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="85671296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1400"/>
+                  <a:t>Values</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1400" baseline="0"/>
+                  <a:t> of n</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="91909120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="91909120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1400"/>
+                  <a:t>Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85671296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr u="none"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" sz="1600" b="1" i="0" u="none" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Sorting Algorithm Times: 2^13 to 2^19</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA" sz="1600" u="none">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15854396325459316"/>
+          <c:y val="8.5692402566093381E-2"/>
+          <c:w val="0.59981671041119855"/>
+          <c:h val="0.77779335474126565"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Method 1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$F$1:$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2^13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$6:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.15615163399999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9734061366666669</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.619648407</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>538.94510173466676</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Method 2</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$F$1:$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2^13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$12:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.14386212200000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9974252459999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.963568778999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>542.95995632166671</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Method 3</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$F$1:$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2^13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$18:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.7045261333333336E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9429221999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8213026333333332E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18189008133333331</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="79492224"/>
+        <c:axId val="79493760"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="79492224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1400"/>
+                  <a:t>Values of n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="79493760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="79493760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="1400"/>
+                  <a:t>Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="79492224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,73 +1256,124 @@
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14">
+      <c r="B3" s="13">
+        <v>3.0357000000000001E-5</v>
+      </c>
+      <c r="C3" s="13">
         <v>3.8627900000000001E-4</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="D3" s="13">
+        <v>5.9147339999999996E-3</v>
+      </c>
+      <c r="E3" s="13">
+        <v>2.4869685999999998E-2</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.16507623499999999</v>
+      </c>
+      <c r="G3" s="13">
+        <v>1.987774575</v>
+      </c>
       <c r="H3" s="3">
         <v>31.472796802000001</v>
       </c>
       <c r="I3" s="1">
-        <v>514.70000000000005</v>
+        <v>529.43359871300004</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14">
+      <c r="B4" s="13">
+        <v>3.0796000000000001E-5</v>
+      </c>
+      <c r="C4" s="13">
         <v>3.8275899999999999E-4</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+      <c r="D4" s="13">
+        <v>4.1021260000000002E-3</v>
+      </c>
+      <c r="E4" s="13">
+        <v>2.4683145E-2</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.17313134199999999</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1.962782142</v>
+      </c>
       <c r="H4" s="3">
         <v>31.899376058000001</v>
       </c>
       <c r="I4" s="1">
-        <v>549.84</v>
+        <v>546.12428727600002</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14">
+      <c r="B5" s="13">
+        <v>2.9916999999999998E-5</v>
+      </c>
+      <c r="C5" s="13">
         <v>3.8363900000000002E-4</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
+      <c r="D5" s="13">
+        <v>4.4263710000000001E-3</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1.8033250000000001E-2</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.130247325</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1.9696616929999999</v>
+      </c>
       <c r="H5" s="3">
         <v>31.486772361</v>
       </c>
       <c r="I5" s="1">
-        <v>547.01</v>
+        <v>541.27741921500001</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="17">
+      <c r="B6" s="15">
+        <f t="shared" ref="B6:H6" si="0">AVERAGE(B3:B5)</f>
+        <v>3.035666666666667E-5</v>
+      </c>
+      <c r="C6" s="15">
+        <f t="shared" si="0"/>
+        <v>3.8422566666666667E-4</v>
+      </c>
+      <c r="D6" s="15">
+        <f t="shared" si="0"/>
+        <v>4.814410333333333E-3</v>
+      </c>
+      <c r="E6" s="15">
+        <f t="shared" si="0"/>
+        <v>2.2528693666666665E-2</v>
+      </c>
+      <c r="F6" s="15">
+        <f t="shared" si="0"/>
+        <v>0.15615163399999998</v>
+      </c>
+      <c r="G6" s="15">
+        <f t="shared" si="0"/>
+        <v>1.9734061366666669</v>
+      </c>
+      <c r="H6" s="15">
+        <f t="shared" si="0"/>
+        <v>31.619648407</v>
+      </c>
+      <c r="I6" s="15">
         <f>AVERAGE(I3:I5)</f>
-        <v>537.18333333333328</v>
+        <v>538.94510173466676</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -642,7 +1388,7 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3"/>
@@ -654,80 +1400,131 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14">
+      <c r="B9" s="13">
+        <v>3.1677000000000002E-5</v>
+      </c>
+      <c r="C9" s="13">
         <v>3.58122E-4</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="D9" s="13">
+        <v>5.6512009999999998E-3</v>
+      </c>
+      <c r="E9" s="13">
+        <v>3.4487068000000003E-2</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0.14612392299999999</v>
+      </c>
+      <c r="G9" s="13">
+        <v>2.006803439</v>
+      </c>
       <c r="H9" s="3">
         <v>32.668425161000002</v>
       </c>
       <c r="I9" s="1">
-        <v>542.5</v>
+        <v>558.88417742800004</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14">
+      <c r="B10" s="13">
+        <v>2.9916999999999998E-5</v>
+      </c>
+      <c r="C10" s="13">
         <v>3.5944200000000002E-4</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="D10" s="13">
+        <v>3.5539429999999999E-3</v>
+      </c>
+      <c r="E10" s="13">
+        <v>2.2536613E-2</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0.13493722699999999</v>
+      </c>
+      <c r="G10" s="13">
+        <v>2.0182831430000001</v>
+      </c>
       <c r="H10" s="3">
         <v>31.550679991999999</v>
       </c>
       <c r="I10" s="1">
-        <v>551.22</v>
+        <v>534.52492731999996</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14">
+      <c r="B11" s="13">
+        <v>2.9476999999999999E-5</v>
+      </c>
+      <c r="C11" s="13">
         <v>3.5856199999999999E-4</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="D11" s="13">
+        <v>3.6406149999999998E-3</v>
+      </c>
+      <c r="E11" s="13">
+        <v>2.3015282000000001E-2</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.15052521599999999</v>
+      </c>
+      <c r="G11" s="13">
+        <v>1.9671891560000001</v>
+      </c>
       <c r="H11" s="3">
         <v>31.671601184</v>
       </c>
       <c r="I11" s="1">
-        <v>519.66</v>
+        <v>535.47076421700001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="17">
+      <c r="B12" s="15">
+        <f t="shared" ref="B12:H12" si="1">AVERAGE(B9:B11)</f>
+        <v>3.0356999999999998E-5</v>
+      </c>
+      <c r="C12" s="15">
+        <f t="shared" si="1"/>
+        <v>3.5870866666666665E-4</v>
+      </c>
+      <c r="D12" s="15">
+        <f t="shared" si="1"/>
+        <v>4.2819196666666667E-3</v>
+      </c>
+      <c r="E12" s="15">
+        <f t="shared" si="1"/>
+        <v>2.6679654333333334E-2</v>
+      </c>
+      <c r="F12" s="15">
+        <f t="shared" si="1"/>
+        <v>0.14386212200000001</v>
+      </c>
+      <c r="G12" s="15">
+        <f t="shared" si="1"/>
+        <v>1.9974252459999999</v>
+      </c>
+      <c r="H12" s="15">
+        <f t="shared" si="1"/>
+        <v>31.963568778999999</v>
+      </c>
+      <c r="I12" s="15">
         <f>AVERAGE(I9:I11)</f>
-        <v>537.79333333333341</v>
+        <v>542.95995632166671</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -738,7 +1535,7 @@
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="3"/>
@@ -750,81 +1547,133 @@
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14">
+      <c r="B15" s="13">
+        <v>9.1949999999999999E-5</v>
+      </c>
+      <c r="C15" s="13">
         <v>2.88609E-4</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="D15" s="13">
+        <v>1.372655E-3</v>
+      </c>
+      <c r="E15" s="13">
+        <v>1.901479E-3</v>
+      </c>
+      <c r="F15" s="13">
+        <v>6.7620839999999998E-3</v>
+      </c>
+      <c r="G15" s="13">
+        <v>1.6898610000000001E-2</v>
+      </c>
       <c r="H15" s="3">
         <v>4.8886302E-2</v>
       </c>
       <c r="I15" s="1">
-        <v>0.18</v>
+        <v>0.18235452499999999</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14">
+      <c r="B16" s="13">
+        <v>8.0951999999999993E-5</v>
+      </c>
+      <c r="C16" s="13">
         <v>2.6397200000000001E-4</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="D16" s="13">
+        <v>1.9617520000000002E-3</v>
+      </c>
+      <c r="E16" s="13">
+        <v>1.859243E-3</v>
+      </c>
+      <c r="F16" s="13">
+        <v>6.7920000000000003E-3</v>
+      </c>
+      <c r="G16" s="13">
+        <v>2.4413454000000001E-2</v>
+      </c>
       <c r="H16" s="3">
         <v>4.7949200999999997E-2</v>
       </c>
       <c r="I16" s="1">
-        <v>0.18</v>
+        <v>0.181540172</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14">
+      <c r="B17" s="13">
+        <v>8.4470999999999998E-5</v>
+      </c>
+      <c r="C17" s="13">
         <v>2.7233100000000001E-4</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="D17" s="13">
+        <v>1.4751639999999999E-3</v>
+      </c>
+      <c r="E17" s="13">
+        <v>2.0035470000000001E-3</v>
+      </c>
+      <c r="F17" s="13">
+        <v>3.7581700000000003E-2</v>
+      </c>
+      <c r="G17" s="13">
+        <v>1.6975601999999999E-2</v>
+      </c>
       <c r="H17" s="3">
         <v>4.7803576E-2</v>
       </c>
       <c r="I17" s="1">
-        <v>0.19</v>
+        <v>0.18177554700000001</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+    <row r="18" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="17">
+      <c r="B18" s="15">
+        <f t="shared" ref="B18:H18" si="2">AVERAGE(B15:B17)</f>
+        <v>8.5790999999999992E-5</v>
+      </c>
+      <c r="C18" s="15">
+        <f t="shared" si="2"/>
+        <v>2.7497066666666667E-4</v>
+      </c>
+      <c r="D18" s="15">
+        <f t="shared" si="2"/>
+        <v>1.6031903333333334E-3</v>
+      </c>
+      <c r="E18" s="15">
+        <f t="shared" si="2"/>
+        <v>1.9214230000000002E-3</v>
+      </c>
+      <c r="F18" s="15">
+        <f t="shared" si="2"/>
+        <v>1.7045261333333336E-2</v>
+      </c>
+      <c r="G18" s="15">
+        <f t="shared" si="2"/>
+        <v>1.9429221999999999E-2</v>
+      </c>
+      <c r="H18" s="15">
+        <f t="shared" si="2"/>
+        <v>4.8213026333333332E-2</v>
+      </c>
+      <c r="I18" s="15">
         <f>AVERAGE(I15:I17)</f>
-        <v>0.18333333333333335</v>
+        <v>0.18189008133333331</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>